<commit_message>
MagicBricks website automation testing successfully completed- with reports
</commit_message>
<xml_diff>
--- a/Reports_files/MagicBricks_TestingApplication-Gopika R.xlsx
+++ b/Reports_files/MagicBricks_TestingApplication-Gopika R.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0740C771D868F598/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5E9A935-8145-4FA8-813A-8AE480A3C143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{B5E9A935-8145-4FA8-813A-8AE480A3C143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16592629-F260-423F-8CBC-0C9A24390688}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{203D3CF5-C1A9-4458-9B77-2F3A8832C505}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{203D3CF5-C1A9-4458-9B77-2F3A8832C505}"/>
   </bookViews>
   <sheets>
     <sheet name="User Story" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="303">
   <si>
     <t>Issue Type</t>
   </si>
@@ -110,9 +110,6 @@
     <t>BR_ID</t>
   </si>
   <si>
-    <t>TR_ID</t>
-  </si>
-  <si>
     <t>TS_ID</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
     <t>RS_1.2</t>
   </si>
   <si>
-    <t>RS_1.3</t>
-  </si>
-  <si>
     <t>RS_2</t>
   </si>
   <si>
@@ -311,21 +305,9 @@
     <t>RS_4</t>
   </si>
   <si>
-    <t>RS_5</t>
-  </si>
-  <si>
-    <t>RS_6.1</t>
-  </si>
-  <si>
-    <t>RS_7.1</t>
-  </si>
-  <si>
     <t>RS_3.2</t>
   </si>
   <si>
-    <t>RS_3.3</t>
-  </si>
-  <si>
     <t>RS_4.1</t>
   </si>
   <si>
@@ -351,9 +333,6 @@
   </si>
   <si>
     <t>Test buying a property</t>
-  </si>
-  <si>
-    <t>RS_7.2</t>
   </si>
   <si>
     <t xml:space="preserve"> Open Google Chrome</t>
@@ -977,18 +956,6 @@
     <t>TS_MB_09_TC_17</t>
   </si>
   <si>
-    <t>TS_MB_09_TC_18</t>
-  </si>
-  <si>
-    <t>TS_MB_10_TC_19</t>
-  </si>
-  <si>
-    <t>TS_MB_10_TC_20</t>
-  </si>
-  <si>
-    <t>TS_MB_11_TC_21</t>
-  </si>
-  <si>
     <t>DR_MB_01</t>
   </si>
   <si>
@@ -1020,6 +987,30 @@
   </si>
   <si>
     <t>DR_MB_11</t>
+  </si>
+  <si>
+    <t>Verify the details of already shortlisted property</t>
+  </si>
+  <si>
+    <t>Verify the details of already shortlisted properties</t>
+  </si>
+  <si>
+    <t>TS_MB_12</t>
+  </si>
+  <si>
+    <t>TS_MB_10_TC_18</t>
+  </si>
+  <si>
+    <t>TS_MB_11_TC_19</t>
+  </si>
+  <si>
+    <t>TS_MB_12_TC_21</t>
+  </si>
+  <si>
+    <t>TS_MB_11_TC_20</t>
+  </si>
+  <si>
+    <t>DR_MB_12</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1280,9 +1271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1307,6 +1295,36 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1325,47 +1343,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1395,10 +1381,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1698,214 +1680,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9356A596-8957-473E-A213-906C47382439}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="82" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="18" customWidth="1"/>
     <col min="3" max="3" width="80.21875" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="40" t="s">
+      <c r="B3" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="43"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="42" t="s">
+      <c r="D12" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="42" t="s">
+      <c r="C13" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="40" t="s">
-        <v>113</v>
+      <c r="C14" s="31" t="s">
+        <v>106</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1916,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1E877E-036D-40A1-A9A8-6D3C63F26E6E}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView zoomScale="87" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="55.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1928,251 +1911,270 @@
     <col min="2" max="2" width="32.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="31" style="2" customWidth="1"/>
     <col min="4" max="4" width="27.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="45.88671875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" style="17" customWidth="1"/>
+    <col min="6" max="6" width="45.88671875" style="18" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="20">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C3" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" s="20">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D4" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="20">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E2" s="21">
+    </row>
+    <row r="6" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="20">
+        <v>2</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" s="20">
         <v>1</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="F7" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="20">
+        <v>1</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E3" s="21">
-        <v>4</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="E4" s="21">
-        <v>3</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" s="21">
+      <c r="D10" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" s="20">
+        <v>2</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="20">
         <v>1</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="E6" s="21">
-        <v>2</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E7" s="21">
-        <v>1</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E8" s="21">
-        <v>1</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E9" s="21">
-        <v>1</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E10" s="45">
-        <v>3</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E11" s="21">
-        <v>2</v>
-      </c>
       <c r="F11" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>244</v>
+      <c r="C12" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="E12" s="21">
+        <v>230</v>
+      </c>
+      <c r="E12" s="20">
+        <v>2</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="20">
         <v>1</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="H12" s="44"/>
+      <c r="F13" s="12" t="s">
+        <v>247</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2185,7 +2187,7 @@
   <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScale="88" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2208,22 +2210,22 @@
   <sheetData>
     <row r="1" spans="1:30" s="13" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>12</v>
@@ -2250,745 +2252,745 @@
     </row>
     <row r="2" spans="1:30" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>58</v>
+        <v>174</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
       <c r="L2" s="12" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="M2" s="12"/>
     </row>
     <row r="3" spans="1:30" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
+        <v>176</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
       <c r="L3" s="12" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:30" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>58</v>
+        <v>178</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>58</v>
+        <v>179</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:30" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="I5" s="34" t="s">
-        <v>58</v>
+        <v>178</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="K5" s="34" t="s">
-        <v>58</v>
+        <v>179</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:30" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="I6" s="35" t="s">
-        <v>60</v>
+        <v>178</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>59</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="K6" s="34" t="s">
-        <v>58</v>
+        <v>215</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="M6" s="12"/>
     </row>
     <row r="7" spans="1:30" s="6" customFormat="1" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>58</v>
+        <v>181</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J7" s="12"/>
-      <c r="K7" s="37"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="12" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:30" s="6" customFormat="1" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>58</v>
+        <v>133</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J8" s="12"/>
-      <c r="K8" s="37"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="12" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:30" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>144</v>
+        <v>112</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="9" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="I9" s="34" t="s">
-        <v>58</v>
+        <v>129</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>58</v>
+        <v>212</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:30" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="H11" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>58</v>
+        <v>124</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J11" s="12"/>
-      <c r="K11" s="37"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="12" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:30" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="H12" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="I12" s="34" t="s">
-        <v>58</v>
+        <v>207</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J12" s="12"/>
-      <c r="K12" s="37"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="12" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="M12" s="12"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="33"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="32"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="32"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
     </row>
     <row r="13" spans="1:30" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>58</v>
+        <v>205</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:30" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="I14" s="34" t="s">
-        <v>58</v>
+        <v>151</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:30" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="I15" s="34" t="s">
-        <v>58</v>
+        <v>201</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:30" ht="38.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>161</v>
+        <v>136</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>154</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I16" s="34" t="s">
-        <v>58</v>
+        <v>140</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="1:13" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>58</v>
+        <v>157</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>58</v>
+        <v>167</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="M18" s="12"/>
     </row>
     <row r="19" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="E19" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>58</v>
+      <c r="I19" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="12" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>58</v>
+        <v>186</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
       <c r="L20" s="12" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="12" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>58</v>
+        <v>190</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>64</v>
+        <v>297</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>58</v>
+        <v>194</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="M22" s="12"/>
     </row>
@@ -3004,7 +3006,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3019,223 +3021,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B9" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="8" t="s">
+      <c r="F9" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3246,461 +3248,394 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEFFAD4-F3F1-4A06-9345-CC696CE7ADA8}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F3:F22"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="C2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="7"/>
       <c r="C3" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="C7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="D16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="D17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>283</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="D22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>289</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>292</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>294</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B29" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3712,8 +3647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7464A19-FE1C-4B26-A5AC-974D61C8F45C}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="107" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3730,64 +3665,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="40"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3">
         <v>21</v>
@@ -3801,13 +3736,13 @@
       <c r="F4" s="3">
         <v>21</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="23">
         <v>0</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="23">
         <v>1</v>
       </c>
     </row>

</xml_diff>